<commit_message>
chuẩn bị làm Use case diagram
</commit_message>
<xml_diff>
--- a/Assignment.xlsx
+++ b/Assignment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -36,10 +36,22 @@
     <t>Ngô Thị Mỹ Linh</t>
   </si>
   <si>
-    <t>Mô tả nghiệp vụ Admin, vẽ sơ đồ usecase Admin, mô tả usecase Admin</t>
-  </si>
-  <si>
-    <t>Mô tả nghiệp vụ User, vẽ sơ đồ usecase User, mô tả usecase User</t>
+    <t>Mô tả nghiệp vụ Admin, vẽ sơ đồ usecase Admin</t>
+  </si>
+  <si>
+    <t>Mô tả nghiệp vụ User, vẽ sơ đồ usecase User</t>
+  </si>
+  <si>
+    <t>week3</t>
+  </si>
+  <si>
+    <t>Mô ta usecae Admin,  vẽ sơ đồ use case, ghi vào file Usecase specification</t>
+  </si>
+  <si>
+    <t>mô tả use case học viên,  vẽ sơ đồ use case, ghi vào file Usecase specification</t>
+  </si>
+  <si>
+    <t>Vẽ flow use case, và bảng Flow UC</t>
   </si>
 </sst>
 </file>
@@ -357,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D5"/>
+  <dimension ref="B3:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -367,9 +379,10 @@
   <cols>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -379,21 +392,36 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>